<commit_message>
1. add json-lib 2. handle output
</commit_message>
<xml_diff>
--- a/info/China_SURF_Station.xlsx
+++ b/info/China_SURF_Station.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\用户目录\Documents\Tencent Files\109907891\FileRecv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding\Github\GraspWeatherInfo\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="23475" windowHeight="9345"/>
+    <workbookView xWindow="1365" yWindow="390" windowWidth="23475" windowHeight="9345"/>
   </bookViews>
   <sheets>
     <sheet name="开放站点" sheetId="1" r:id="rId1"/>
@@ -7625,7 +7625,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7814,6 +7814,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8170,7 +8176,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="297">
+  <cellXfs count="306">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -9066,6 +9072,33 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="33" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="177" fontId="33" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="177" fontId="33" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="177" fontId="33" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="99">
     <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -9257,23 +9290,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -9309,23 +9325,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -9504,8 +9503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A668" workbookViewId="0">
+      <selection activeCell="A641" sqref="A641"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -26134,54 +26133,54 @@
       </c>
     </row>
     <row r="640" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A640" s="48">
+      <c r="A640" s="297">
         <v>54398</v>
       </c>
-      <c r="B640" s="10" t="s">
+      <c r="B640" s="298" t="s">
         <v>24</v>
       </c>
-      <c r="C640" s="10" t="s">
+      <c r="C640" s="298" t="s">
         <v>25</v>
       </c>
-      <c r="D640" s="10" t="s">
+      <c r="D640" s="298" t="s">
         <v>26</v>
       </c>
-      <c r="E640" s="49">
+      <c r="E640" s="299">
         <v>11637</v>
       </c>
-      <c r="F640" s="48">
+      <c r="F640" s="297">
         <v>4008</v>
       </c>
-      <c r="G640" s="11">
+      <c r="G640" s="300">
         <v>28.6</v>
       </c>
-      <c r="H640" s="11">
+      <c r="H640" s="300">
         <v>29.6</v>
       </c>
     </row>
     <row r="641" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A641" s="48">
+      <c r="A641" s="297">
         <v>54399</v>
       </c>
-      <c r="B641" s="10" t="s">
+      <c r="B641" s="298" t="s">
         <v>24</v>
       </c>
-      <c r="C641" s="10" t="s">
+      <c r="C641" s="298" t="s">
         <v>27</v>
       </c>
-      <c r="D641" s="10" t="s">
+      <c r="D641" s="298" t="s">
         <v>26</v>
       </c>
-      <c r="E641" s="49">
+      <c r="E641" s="299">
         <v>11617</v>
       </c>
-      <c r="F641" s="48">
+      <c r="F641" s="297">
         <v>3959</v>
       </c>
-      <c r="G641" s="11">
+      <c r="G641" s="300">
         <v>45.8</v>
       </c>
-      <c r="H641" s="11">
+      <c r="H641" s="300">
         <v>46.9</v>
       </c>
     </row>
@@ -26264,28 +26263,28 @@
       </c>
     </row>
     <row r="645" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A645" s="48">
+      <c r="A645" s="297">
         <v>54406</v>
       </c>
-      <c r="B645" s="10" t="s">
+      <c r="B645" s="298" t="s">
         <v>24</v>
       </c>
-      <c r="C645" s="10" t="s">
+      <c r="C645" s="298" t="s">
         <v>28</v>
       </c>
-      <c r="D645" s="10" t="s">
+      <c r="D645" s="298" t="s">
         <v>29</v>
       </c>
-      <c r="E645" s="49">
+      <c r="E645" s="299">
         <v>11558</v>
       </c>
-      <c r="F645" s="48">
+      <c r="F645" s="297">
         <v>4027</v>
       </c>
-      <c r="G645" s="11">
+      <c r="G645" s="300">
         <v>487.9</v>
       </c>
-      <c r="H645" s="11">
+      <c r="H645" s="300">
         <v>489.1</v>
       </c>
     </row>
@@ -26316,54 +26315,54 @@
       </c>
     </row>
     <row r="647" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A647" s="48">
+      <c r="A647" s="297">
         <v>54416</v>
       </c>
-      <c r="B647" s="10" t="s">
+      <c r="B647" s="298" t="s">
         <v>30</v>
       </c>
-      <c r="C647" s="10" t="s">
+      <c r="C647" s="298" t="s">
         <v>32</v>
       </c>
-      <c r="D647" s="10" t="s">
+      <c r="D647" s="298" t="s">
         <v>33</v>
       </c>
-      <c r="E647" s="49">
+      <c r="E647" s="299">
         <v>11652</v>
       </c>
-      <c r="F647" s="48">
+      <c r="F647" s="297">
         <v>4023</v>
       </c>
-      <c r="G647" s="11">
+      <c r="G647" s="300">
         <v>71.8</v>
       </c>
-      <c r="H647" s="11">
+      <c r="H647" s="300">
         <v>73</v>
       </c>
     </row>
     <row r="648" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A648" s="48">
+      <c r="A648" s="297">
         <v>54419</v>
       </c>
-      <c r="B648" s="10" t="s">
+      <c r="B648" s="298" t="s">
         <v>30</v>
       </c>
-      <c r="C648" s="10" t="s">
+      <c r="C648" s="298" t="s">
         <v>34</v>
       </c>
-      <c r="D648" s="10" t="s">
+      <c r="D648" s="298" t="s">
         <v>31</v>
       </c>
-      <c r="E648" s="49">
+      <c r="E648" s="299">
         <v>11638</v>
       </c>
-      <c r="F648" s="48">
+      <c r="F648" s="297">
         <v>4022</v>
       </c>
-      <c r="G648" s="11">
+      <c r="G648" s="300">
         <v>75.7</v>
       </c>
-      <c r="H648" s="8">
+      <c r="H648" s="301">
         <v>76.8</v>
       </c>
     </row>
@@ -26394,28 +26393,28 @@
       </c>
     </row>
     <row r="650" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A650" s="48">
+      <c r="A650" s="297">
         <v>54421</v>
       </c>
-      <c r="B650" s="10" t="s">
+      <c r="B650" s="298" t="s">
         <v>30</v>
       </c>
-      <c r="C650" s="10" t="s">
+      <c r="C650" s="298" t="s">
         <v>35</v>
       </c>
-      <c r="D650" s="10" t="s">
+      <c r="D650" s="298" t="s">
         <v>31</v>
       </c>
-      <c r="E650" s="49">
+      <c r="E650" s="299">
         <v>11707</v>
       </c>
-      <c r="F650" s="48">
+      <c r="F650" s="297">
         <v>4039</v>
       </c>
-      <c r="G650" s="11">
+      <c r="G650" s="300">
         <v>293.3</v>
       </c>
-      <c r="H650" s="11">
+      <c r="H650" s="300">
         <v>294.3</v>
       </c>
     </row>
@@ -26446,28 +26445,28 @@
       </c>
     </row>
     <row r="652" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A652" s="48">
+      <c r="A652" s="297">
         <v>54424</v>
       </c>
-      <c r="B652" s="10" t="s">
+      <c r="B652" s="298" t="s">
         <v>30</v>
       </c>
-      <c r="C652" s="10" t="s">
+      <c r="C652" s="298" t="s">
         <v>36</v>
       </c>
-      <c r="D652" s="10" t="s">
+      <c r="D652" s="298" t="s">
         <v>31</v>
       </c>
-      <c r="E652" s="50">
+      <c r="E652" s="302">
         <v>11707</v>
       </c>
-      <c r="F652" s="48">
+      <c r="F652" s="297">
         <v>4010</v>
       </c>
-      <c r="G652" s="11">
+      <c r="G652" s="300">
         <v>32.1</v>
       </c>
-      <c r="H652" s="8">
+      <c r="H652" s="301">
         <v>33.299999999999997</v>
       </c>
     </row>
@@ -26576,28 +26575,28 @@
       </c>
     </row>
     <row r="657" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A657" s="48">
+      <c r="A657" s="297">
         <v>54431</v>
       </c>
-      <c r="B657" s="10" t="s">
+      <c r="B657" s="298" t="s">
         <v>30</v>
       </c>
-      <c r="C657" s="10" t="s">
+      <c r="C657" s="298" t="s">
         <v>37</v>
       </c>
-      <c r="D657" s="10" t="s">
+      <c r="D657" s="298" t="s">
         <v>31</v>
       </c>
-      <c r="E657" s="50">
+      <c r="E657" s="302">
         <v>11645</v>
       </c>
-      <c r="F657" s="48">
+      <c r="F657" s="297">
         <v>3951</v>
       </c>
-      <c r="G657" s="11">
+      <c r="G657" s="300">
         <v>19.8</v>
       </c>
-      <c r="H657" s="11">
+      <c r="H657" s="300">
         <v>20.8</v>
       </c>
     </row>
@@ -26628,28 +26627,28 @@
       </c>
     </row>
     <row r="659" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A659" s="48">
+      <c r="A659" s="297">
         <v>54433</v>
       </c>
-      <c r="B659" s="10" t="s">
+      <c r="B659" s="298" t="s">
         <v>30</v>
       </c>
-      <c r="C659" s="10" t="s">
+      <c r="C659" s="298" t="s">
         <v>38</v>
       </c>
-      <c r="D659" s="10" t="s">
+      <c r="D659" s="298" t="s">
         <v>31</v>
       </c>
-      <c r="E659" s="50">
+      <c r="E659" s="302">
         <v>11630</v>
       </c>
-      <c r="F659" s="48">
+      <c r="F659" s="297">
         <v>3957</v>
       </c>
-      <c r="G659" s="6">
+      <c r="G659" s="303">
         <v>35.299999999999997</v>
       </c>
-      <c r="H659" s="11">
+      <c r="H659" s="300">
         <v>36.299999999999997</v>
       </c>
     </row>
@@ -27174,54 +27173,54 @@
       </c>
     </row>
     <row r="680" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A680" s="48">
+      <c r="A680" s="297">
         <v>54499</v>
       </c>
-      <c r="B680" s="10" t="s">
+      <c r="B680" s="298" t="s">
         <v>30</v>
       </c>
-      <c r="C680" s="10" t="s">
+      <c r="C680" s="298" t="s">
         <v>39</v>
       </c>
-      <c r="D680" s="10" t="s">
+      <c r="D680" s="298" t="s">
         <v>31</v>
       </c>
-      <c r="E680" s="49">
+      <c r="E680" s="299">
         <v>11613</v>
       </c>
-      <c r="F680" s="48">
+      <c r="F680" s="297">
         <v>4013</v>
       </c>
-      <c r="G680" s="11">
+      <c r="G680" s="300">
         <v>76.2</v>
       </c>
-      <c r="H680" s="11">
+      <c r="H680" s="300">
         <v>77.400000000000006</v>
       </c>
     </row>
     <row r="681" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A681" s="48">
+      <c r="A681" s="297">
         <v>54501</v>
       </c>
-      <c r="B681" s="10" t="s">
+      <c r="B681" s="298" t="s">
         <v>30</v>
       </c>
-      <c r="C681" s="10" t="s">
+      <c r="C681" s="298" t="s">
         <v>40</v>
       </c>
-      <c r="D681" s="10" t="s">
+      <c r="D681" s="298" t="s">
         <v>31</v>
       </c>
-      <c r="E681" s="49">
+      <c r="E681" s="299">
         <v>11541</v>
       </c>
-      <c r="F681" s="48">
+      <c r="F681" s="297">
         <v>3958</v>
       </c>
-      <c r="G681" s="11">
+      <c r="G681" s="300">
         <v>440.3</v>
       </c>
-      <c r="H681" s="11">
+      <c r="H681" s="300">
         <v>441.3</v>
       </c>
     </row>
@@ -27278,28 +27277,28 @@
       </c>
     </row>
     <row r="684" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A684" s="4">
+      <c r="A684" s="304">
         <v>54505</v>
       </c>
-      <c r="B684" s="4" t="s">
+      <c r="B684" s="304" t="s">
         <v>30</v>
       </c>
-      <c r="C684" s="4" t="s">
+      <c r="C684" s="304" t="s">
         <v>41</v>
       </c>
-      <c r="D684" s="4" t="s">
+      <c r="D684" s="304" t="s">
         <v>31</v>
       </c>
-      <c r="E684" s="14">
+      <c r="E684" s="305">
         <v>11609</v>
       </c>
-      <c r="F684" s="14">
+      <c r="F684" s="305">
         <v>3953</v>
       </c>
-      <c r="G684" s="6">
+      <c r="G684" s="303">
         <v>85.5</v>
       </c>
-      <c r="H684" s="6">
+      <c r="H684" s="303">
         <v>86.6</v>
       </c>
     </row>
@@ -27382,28 +27381,28 @@
       </c>
     </row>
     <row r="688" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A688" s="48">
+      <c r="A688" s="297">
         <v>54511</v>
       </c>
-      <c r="B688" s="10" t="s">
+      <c r="B688" s="298" t="s">
         <v>30</v>
       </c>
-      <c r="C688" s="10" t="s">
+      <c r="C688" s="298" t="s">
         <v>30</v>
       </c>
-      <c r="D688" s="10" t="s">
+      <c r="D688" s="298" t="s">
         <v>29</v>
       </c>
-      <c r="E688" s="49">
+      <c r="E688" s="299">
         <v>11628</v>
       </c>
-      <c r="F688" s="48">
+      <c r="F688" s="297">
         <v>3948</v>
       </c>
-      <c r="G688" s="11">
+      <c r="G688" s="300">
         <v>31.3</v>
       </c>
-      <c r="H688" s="11">
+      <c r="H688" s="300">
         <v>32.299999999999997</v>
       </c>
     </row>
@@ -27434,54 +27433,54 @@
       </c>
     </row>
     <row r="690" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A690" s="48">
+      <c r="A690" s="297">
         <v>54513</v>
       </c>
-      <c r="B690" s="10" t="s">
+      <c r="B690" s="298" t="s">
         <v>30</v>
       </c>
-      <c r="C690" s="10" t="s">
+      <c r="C690" s="298" t="s">
         <v>42</v>
       </c>
-      <c r="D690" s="10" t="s">
+      <c r="D690" s="298" t="s">
         <v>31</v>
       </c>
-      <c r="E690" s="49">
+      <c r="E690" s="299">
         <v>11612</v>
       </c>
-      <c r="F690" s="48">
+      <c r="F690" s="297">
         <v>3957</v>
       </c>
-      <c r="G690" s="11">
+      <c r="G690" s="300">
         <v>63</v>
       </c>
-      <c r="H690" s="11">
+      <c r="H690" s="300">
         <v>64.099999999999994</v>
       </c>
     </row>
     <row r="691" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A691" s="48">
+      <c r="A691" s="297">
         <v>54514</v>
       </c>
-      <c r="B691" s="10" t="s">
+      <c r="B691" s="298" t="s">
         <v>30</v>
       </c>
-      <c r="C691" s="10" t="s">
+      <c r="C691" s="298" t="s">
         <v>43</v>
       </c>
-      <c r="D691" s="10" t="s">
+      <c r="D691" s="298" t="s">
         <v>31</v>
       </c>
-      <c r="E691" s="49">
+      <c r="E691" s="299">
         <v>11615</v>
       </c>
-      <c r="F691" s="48">
+      <c r="F691" s="297">
         <v>3952</v>
       </c>
-      <c r="G691" s="11">
+      <c r="G691" s="300">
         <v>55.2</v>
       </c>
-      <c r="H691" s="11">
+      <c r="H691" s="300">
         <v>56.7</v>
       </c>
     </row>
@@ -28240,54 +28239,54 @@
       </c>
     </row>
     <row r="721" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A721" s="48">
+      <c r="A721" s="297">
         <v>54594</v>
       </c>
-      <c r="B721" s="10" t="s">
+      <c r="B721" s="298" t="s">
         <v>30</v>
       </c>
-      <c r="C721" s="10" t="s">
+      <c r="C721" s="298" t="s">
         <v>44</v>
       </c>
-      <c r="D721" s="10" t="s">
+      <c r="D721" s="298" t="s">
         <v>31</v>
       </c>
-      <c r="E721" s="49">
+      <c r="E721" s="299">
         <v>11621</v>
       </c>
-      <c r="F721" s="48">
+      <c r="F721" s="297">
         <v>3943</v>
       </c>
-      <c r="G721" s="11">
+      <c r="G721" s="300">
         <v>37.5</v>
       </c>
-      <c r="H721" s="11">
+      <c r="H721" s="300">
         <v>38.700000000000003</v>
       </c>
     </row>
     <row r="722" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A722" s="4">
+      <c r="A722" s="304">
         <v>54596</v>
       </c>
-      <c r="B722" s="4" t="s">
+      <c r="B722" s="304" t="s">
         <v>30</v>
       </c>
-      <c r="C722" s="4" t="s">
+      <c r="C722" s="304" t="s">
         <v>45</v>
       </c>
-      <c r="D722" s="4" t="s">
+      <c r="D722" s="304" t="s">
         <v>31</v>
       </c>
-      <c r="E722" s="4">
+      <c r="E722" s="304">
         <v>11612</v>
       </c>
-      <c r="F722" s="4">
+      <c r="F722" s="304">
         <v>3946</v>
       </c>
-      <c r="G722" s="6">
+      <c r="G722" s="303">
         <v>48.9</v>
       </c>
-      <c r="H722" s="6">
+      <c r="H722" s="303">
         <v>49.9</v>
       </c>
     </row>

</xml_diff>